<commit_message>
Classes for working with xls files were added.
</commit_message>
<xml_diff>
--- a/ConverterToXml.Test/Files/xlsx.xlsx
+++ b/ConverterToXml.Test/Files/xlsx.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipetr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\C#\ConverterToXml\ConverterToXml.Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B99A291-A667-4C75-A33B-C3F07C9ADCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D218514-1880-4C49-BA88-CCEAA60201CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{1149AE9A-75AA-4D53-8476-15DD2417A899}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{1149AE9A-75AA-4D53-8476-15DD2417A899}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="My parent's accounting" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5469,42 +5469,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="O4:P5"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="M18:N19"/>
+    <mergeCell ref="G33:H34"/>
+    <mergeCell ref="O35:P36"/>
+    <mergeCell ref="I38:J39"/>
+    <mergeCell ref="K42:L43"/>
+    <mergeCell ref="G48:H49"/>
+    <mergeCell ref="M49:N50"/>
+    <mergeCell ref="G64:H65"/>
+    <mergeCell ref="O66:P67"/>
+    <mergeCell ref="I69:J70"/>
+    <mergeCell ref="K73:L74"/>
+    <mergeCell ref="G79:H80"/>
+    <mergeCell ref="M80:N81"/>
+    <mergeCell ref="W2:X3"/>
+    <mergeCell ref="AE4:AF5"/>
+    <mergeCell ref="Y7:Z8"/>
+    <mergeCell ref="AA11:AB12"/>
+    <mergeCell ref="W17:X18"/>
+    <mergeCell ref="AC18:AD19"/>
+    <mergeCell ref="W33:X34"/>
+    <mergeCell ref="AE35:AF36"/>
+    <mergeCell ref="Y38:Z39"/>
+    <mergeCell ref="AA42:AB43"/>
+    <mergeCell ref="W48:X49"/>
+    <mergeCell ref="AC49:AD50"/>
     <mergeCell ref="W64:X65"/>
     <mergeCell ref="AE66:AF67"/>
     <mergeCell ref="Y69:Z70"/>
     <mergeCell ref="AA73:AB74"/>
     <mergeCell ref="W79:X80"/>
     <mergeCell ref="AC80:AD81"/>
-    <mergeCell ref="W33:X34"/>
-    <mergeCell ref="AE35:AF36"/>
-    <mergeCell ref="Y38:Z39"/>
-    <mergeCell ref="AA42:AB43"/>
-    <mergeCell ref="W48:X49"/>
-    <mergeCell ref="AC49:AD50"/>
-    <mergeCell ref="W2:X3"/>
-    <mergeCell ref="AE4:AF5"/>
-    <mergeCell ref="Y7:Z8"/>
-    <mergeCell ref="AA11:AB12"/>
-    <mergeCell ref="W17:X18"/>
-    <mergeCell ref="AC18:AD19"/>
-    <mergeCell ref="G64:H65"/>
-    <mergeCell ref="O66:P67"/>
-    <mergeCell ref="I69:J70"/>
-    <mergeCell ref="K73:L74"/>
-    <mergeCell ref="G79:H80"/>
-    <mergeCell ref="M80:N81"/>
-    <mergeCell ref="G33:H34"/>
-    <mergeCell ref="O35:P36"/>
-    <mergeCell ref="I38:J39"/>
-    <mergeCell ref="K42:L43"/>
-    <mergeCell ref="G48:H49"/>
-    <mergeCell ref="M49:N50"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="O4:P5"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="G17:H18"/>
-    <mergeCell ref="M18:N19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>